<commit_message>
Still not finished but closer
</commit_message>
<xml_diff>
--- a/fitts_law_results.xlsx
+++ b/fitts_law_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,18 +472,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>291.0068727710739</v>
+        <v>178.0589789929168</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -494,18 +494,18 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>191.0104709171725</v>
+        <v>178.0589789929168</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -516,7 +516,1173 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>303.3562262423503</v>
+        <v>350.0014285685131</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>100</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>518.0086871858425</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>518.0086871858425</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9.219544457292887</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.082762530298219</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>426.0105632493166</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>426.0105632493166</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>107.2287274940816</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>391.0051150560565</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" t="n">
+        <v>100</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>306.0065358779123</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>287.0017421549911</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10</v>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>246.1645790929312</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>217.2302925468729</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>310.3626910567699</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>448.0546841625473</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>26.47640458974745</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>26.47640458974745</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>277.0288793609793</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>10</v>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>466.0268232623526</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>16.49242250247064</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>16.49242250247064</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>296.108088373148</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>10</v>
+      </c>
+      <c r="C27" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>343.0364412128834</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="n">
+        <v>175.071414000116</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>10</v>
+      </c>
+      <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>203.0098519776811</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
+        <v>463.8458795763955</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>10</v>
+      </c>
+      <c r="C31" t="n">
+        <v>100</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>212.0212253525576</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0</v>
+      </c>
+      <c r="B32" t="n">
+        <v>10</v>
+      </c>
+      <c r="C32" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>215.00930212435</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>10</v>
+      </c>
+      <c r="C33" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
+        <v>456.4832965180654</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" t="n">
+        <v>10</v>
+      </c>
+      <c r="C34" t="n">
+        <v>100</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="n">
+        <v>13.60147050873544</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0</v>
+      </c>
+      <c r="B35" t="n">
+        <v>10</v>
+      </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="n">
+        <v>481.0093554183744</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0</v>
+      </c>
+      <c r="B36" t="n">
+        <v>10</v>
+      </c>
+      <c r="C36" t="n">
+        <v>100</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>481.0093554183744</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0</v>
+      </c>
+      <c r="B37" t="n">
+        <v>10</v>
+      </c>
+      <c r="C37" t="n">
+        <v>100</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
+        <v>52.03844732503075</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0</v>
+      </c>
+      <c r="B38" t="n">
+        <v>10</v>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>188.0425483766905</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0</v>
+      </c>
+      <c r="B39" t="n">
+        <v>10</v>
+      </c>
+      <c r="C39" t="n">
+        <v>100</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>300.0016666620371</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>10</v>
+      </c>
+      <c r="C40" t="n">
+        <v>100</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="n">
+        <v>300.0016666620371</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>10</v>
+      </c>
+      <c r="C41" t="n">
+        <v>100</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="n">
+        <v>195.0922858546693</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>10</v>
+      </c>
+      <c r="C42" t="n">
+        <v>100</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>190.1289036417135</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0</v>
+      </c>
+      <c r="B43" t="n">
+        <v>10</v>
+      </c>
+      <c r="C43" t="n">
+        <v>100</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="n">
+        <v>365.0671171168392</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0</v>
+      </c>
+      <c r="B44" t="n">
+        <v>10</v>
+      </c>
+      <c r="C44" t="n">
+        <v>100</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>365.0671171168392</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0</v>
+      </c>
+      <c r="B45" t="n">
+        <v>10</v>
+      </c>
+      <c r="C45" t="n">
+        <v>100</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>184.0108692441835</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0</v>
+      </c>
+      <c r="B46" t="n">
+        <v>10</v>
+      </c>
+      <c r="C46" t="n">
+        <v>100</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="n">
+        <v>184.0108692441835</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0</v>
+      </c>
+      <c r="B47" t="n">
+        <v>10</v>
+      </c>
+      <c r="C47" t="n">
+        <v>100</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>47.09564735726646</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0</v>
+      </c>
+      <c r="B48" t="n">
+        <v>10</v>
+      </c>
+      <c r="C48" t="n">
+        <v>100</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="n">
+        <v>47.09564735726646</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0</v>
+      </c>
+      <c r="B49" t="n">
+        <v>10</v>
+      </c>
+      <c r="C49" t="n">
+        <v>100</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="n">
+        <v>79.05694150420949</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0</v>
+      </c>
+      <c r="B50" t="n">
+        <v>10</v>
+      </c>
+      <c r="C50" t="n">
+        <v>100</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>240.0520776831561</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0</v>
+      </c>
+      <c r="B51" t="n">
+        <v>10</v>
+      </c>
+      <c r="C51" t="n">
+        <v>100</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0</v>
+      </c>
+      <c r="B52" t="n">
+        <v>10</v>
+      </c>
+      <c r="C52" t="n">
+        <v>100</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0</v>
+      </c>
+      <c r="B53" t="n">
+        <v>10</v>
+      </c>
+      <c r="C53" t="n">
+        <v>100</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>507.0039447578293</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0</v>
+      </c>
+      <c r="B54" t="n">
+        <v>10</v>
+      </c>
+      <c r="C54" t="n">
+        <v>100</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="n">
+        <v>507.0039447578293</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>10</v>
+      </c>
+      <c r="C55" t="n">
+        <v>100</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" t="n">
+        <v>318.0062892459833</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>10</v>
+      </c>
+      <c r="C56" t="n">
+        <v>100</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>177.0451919708638</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>10</v>
+      </c>
+      <c r="C57" t="n">
+        <v>100</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>left</t>
+        </is>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" t="n">
+        <v>255.3311575190149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>